<commit_message>
#355 final testing and changes to CSV Schema generation
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/parsers/data.xlsx
+++ b/dsl/src/test/data/parsers/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\parsers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1319DA1-D50B-48BB-804C-C000B0A2519D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC2BD6A-8AD4-4963-B724-8E62D489D85C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="754" yWindow="754" windowWidth="16457" windowHeight="8743" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataSheet" sheetId="1" r:id="rId1"/>
@@ -931,7 +931,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -992,10 +992,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412C0CD6-D03F-4052-B7C4-D6E681DC6E66}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1062,6 +1062,20 @@
       </c>
       <c r="E4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <v>444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>